<commit_message>
Added the missing constraints
Found a mistake in AffineFlowThinning python file - constraints of type 3 were missing, and there were double constraints of type 4
File has been corrected, the results of AFT for the small example are now different. 
Added some new comments in FlowThinning python file and AffineFlowThinning python file.
</commit_message>
<xml_diff>
--- a/Results_AffineFlowThinning.xlsx
+++ b/Results_AffineFlowThinning.xlsx
@@ -382,7 +382,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -395,7 +395,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -408,7 +408,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>8.75</v>
       </c>
     </row>
   </sheetData>
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>7.75</v>
       </c>
     </row>
     <row r="5">
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -1309,7 +1309,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -1348,7 +1348,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="6">
@@ -1426,7 +1426,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">

</xml_diff>